<commit_message>
Added data to calculator.xlsx
</commit_message>
<xml_diff>
--- a/docs/calculator.xlsx
+++ b/docs/calculator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="BLEU_Compile" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="COMPILE_freq" sheetId="4" r:id="rId3"/>
     <sheet name="compile_compile" sheetId="3" r:id="rId4"/>
     <sheet name="last" sheetId="5" r:id="rId5"/>
+    <sheet name="APR Fixes" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="blue_calculator_compile_model" localSheetId="0">BLEU_Compile!$A$1:$C$24</definedName>
@@ -24,6 +25,7 @@
     <definedName name="compile_calculator_compile_model" localSheetId="3">compile_compile!$A$1:$G$17</definedName>
     <definedName name="compile_calculator_compile_model" localSheetId="4">last!$A$1:$G$17</definedName>
     <definedName name="compile_calculator_freq_param" localSheetId="2">COMPILE_freq!$A$1:$G$17</definedName>
+    <definedName name="compile_calculator_import_fixes" localSheetId="5">'APR Fixes'!$A$1:$G$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -93,11 +95,24 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="6" name="compile_calculator_import_fixes" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="866" sourceFile="C:\Users\Ivan\PycharmProjects\auto-test-generator\compile_calculator_import_fixes.csv" decimal="," thousands=" " comma="1">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="116">
   <si>
     <t>commit-hash</t>
   </si>
@@ -397,6 +412,54 @@
   </si>
   <si>
     <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/gen_tests_model_last/test_test_f491b817-a7c0-48ed-94be-6a948abe080e.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_20cf42f6-2a5c-4f42-905e-1e405a6819e4.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_cdacc555-a90f-4e9b-948b-d876ba3f1203.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_d3d0481b-cb04-4577-9a1b-74147a9fd1ff.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_2b5ec2c9-f4e2-422f-b487-947be32fc752.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_ca9170fd-cc34-42c5-a754-bc71f9d098c1.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_b301d903-d0e2-47de-bb96-0635e9a8f2ad.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_0732f07b-2b4a-405c-8f2a-7207beac0373.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_892ce0e9-cd73-4ccd-80df-b4d809cb6d28.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_963bd1c4-f2fa-45c4-b5c5-a3fcf3fd3028.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_832ec579-2bfc-4180-9ad6-d6ff038572c7.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_fc0acdb6-6a62-4379-889e-33cab57cef55.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_0261b4c8-c104-4e92-83d0-5850dfe66db4.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_551e2a08-0c23-44bd-95b9-54ad118a11ad.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_d044855c-4c78-422d-ace6-7117203b0c3c.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_0189b152-3a69-49e7-a906-33d4eeba9694.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_2bff72c1-cffc-4771-adbc-28587ff3a3d1.py</t>
   </si>
 </sst>
 </file>
@@ -470,6 +533,10 @@
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="compile_calculator_compile_model" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="compile_calculator_import_fixes" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1731,7 +1798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -2167,7 +2234,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G18" sqref="C18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2593,5 +2660,440 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="140.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f>1-SUM(C2:C17)/COUNT(C2:C17)</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f>SUM(D2:D17)</f>
+        <v>14</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E18:G18" si="0">SUM(E2:E17)</f>
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Coverage in results.
</commit_message>
<xml_diff>
--- a/docs/calculator.xlsx
+++ b/docs/calculator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="BLEU_Compile" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="compile_compile" sheetId="3" r:id="rId4"/>
     <sheet name="last" sheetId="5" r:id="rId5"/>
     <sheet name="APR Fixes" sheetId="6" r:id="rId6"/>
+    <sheet name="Coverage_compilation" sheetId="7" r:id="rId7"/>
+    <sheet name="Coverage" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="blue_calculator_compile_model" localSheetId="0">BLEU_Compile!$A$1:$C$24</definedName>
@@ -26,6 +28,8 @@
     <definedName name="compile_calculator_compile_model" localSheetId="4">last!$A$1:$G$17</definedName>
     <definedName name="compile_calculator_freq_param" localSheetId="2">COMPILE_freq!$A$1:$G$17</definedName>
     <definedName name="compile_calculator_import_fixes" localSheetId="5">'APR Fixes'!$A$1:$G$17</definedName>
+    <definedName name="compile_pydriller_import_fixes" localSheetId="6">Coverage_compilation!$A$1:$G$17</definedName>
+    <definedName name="coverage_compile_pydriller_import_fixes_1" localSheetId="7">Coverage!$A$1:$E$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -108,11 +112,35 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="7" name="compile_pydriller_import_fixes" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="866" sourceFile="C:\Users\Ivan\PycharmProjects\auto-test-generator\compile_pydriller_import_fixes.csv" decimal="," thousands=" " comma="1">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="8" name="coverage_compile_pydriller_import_fixes" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="866" sourceFile="C:\Users\Ivan\PycharmProjects\auto-test-generator\coverage_compile_pydriller_import_fixes.csv" decimal="," thousands=" " comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="137">
   <si>
     <t>commit-hash</t>
   </si>
@@ -460,6 +488,69 @@
   </si>
   <si>
     <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\calculator/get_tests_imports_fixes/test_2bff72c1-cffc-4771-adbc-28587ff3a3d1.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_a585ded6-7a08-47c7-8e56-f53bc99bb94d.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_f3506955-a8e9-4601-9968-0a103e8ac476.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_79b787ff-cb96-499c-927f-82dc5180ad9b.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_e8c5c0a3-754b-42c1-bbfb-6487a8dd3c41.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_5027d7fb-a798-4120-9df9-3df881c68949.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_05f22037-b9ce-40fe-8d4e-e0014c8c66cf.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_46442259-4a32-4923-9bdf-83fc47577a59.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_d1fce6f6-0c61-4dde-aecd-89788b8756f1.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_0870e334-93be-4b22-a2b8-6b3b0ef00893.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_7ec3bc5f-493a-4ea2-bcd5-ddd963170c44.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_8dce3703-5bff-4160-815e-585706fac496.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_fdf7f1eb-0ecc-499e-8857-fd943c6ddd1e.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_905f8521-4b2a-4cf3-9763-c8ba83f12b03.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_2f1e9b13-3448-4cc1-ab4d-251732319722.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_e518c9e9-2867-42a4-835b-b21de82b376b.py</t>
+  </si>
+  <si>
+    <t>C:\Users\Ivan\PycharmProjects\auto-test-generator\dataset_repos\fake-calculator/gen_tests_evaluation/test_9cd8aabd-0cac-4105-a07d-2f2d50a765a4.py</t>
+  </si>
+  <si>
+    <t>Commit_id</t>
+  </si>
+  <si>
+    <t>Statements</t>
+  </si>
+  <si>
+    <t>Misses</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Coverage</t>
   </si>
 </sst>
 </file>
@@ -537,6 +628,14 @@
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="compile_calculator_import_fixes" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="compile_pydriller_import_fixes" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="coverage_compile_pydriller_import_fixes_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2668,8 +2767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3095,5 +3194,686 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f>1-SUM(C2:C17)/COUNT(C2:C17)</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f>SUM(D2:D17)</f>
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E18:G18" si="0">SUM(E2:E17)</f>
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="43.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="7" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>63</v>
+      </c>
+      <c r="D2">
+        <v>41</v>
+      </c>
+      <c r="E2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>63</v>
+      </c>
+      <c r="D3">
+        <v>41</v>
+      </c>
+      <c r="E3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>63</v>
+      </c>
+      <c r="D4">
+        <v>41</v>
+      </c>
+      <c r="E4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>83</v>
+      </c>
+      <c r="D5">
+        <v>48</v>
+      </c>
+      <c r="E5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>128</v>
+      </c>
+      <c r="D6">
+        <v>78</v>
+      </c>
+      <c r="E6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>68</v>
+      </c>
+      <c r="D8">
+        <v>53</v>
+      </c>
+      <c r="E8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11">
+        <v>37</v>
+      </c>
+      <c r="D11">
+        <v>28</v>
+      </c>
+      <c r="E11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13">
+        <f>AVERAGE(C2:C12)</f>
+        <v>53.81818181818182</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:E13" si="0">AVERAGE(D2:D12)</f>
+        <v>33.545454545454547</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>38.909090909090907</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added latest docs and data for httpie.
</commit_message>
<xml_diff>
--- a/docs/calculator.xlsx
+++ b/docs/calculator.xlsx
@@ -3203,7 +3203,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C18" sqref="C18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3636,8 +3636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>